<commit_message>
about same length with encoding error
</commit_message>
<xml_diff>
--- a/web_sum_output.xlsx
+++ b/web_sum_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>URL</t>
   </si>
@@ -55,50 +55,47 @@
     <t>arxiv</t>
   </si>
   <si>
-    <t>youtube</t>
-  </si>
-  <si>
     <t>google</t>
   </si>
   <si>
-    <t>打造自己的变异禀赋</t>
-  </si>
-  <si>
-    <t>AV 2.0，自动驾驶车辆的下一个重要革新</t>
-  </si>
-  <si>
-    <t>欢迎进入基于AWS上的云端生成式人工智能建筑的新时代。</t>
-  </si>
-  <si>
-    <t>微软云玺主权版现已通用，为政府创新打开了新的道路。</t>
-  </si>
-  <si>
-    <t>迈向强人工智能的先驱研究</t>
-  </si>
-  <si>
-    <t>垂直告断段-
-犬癌治疗公司ImpriMed旨在将其人工智能技术扩展到人类肿瘤学。</t>
-  </si>
-  <si>
-    <t>ProlificDreamer：高保真和多样化的文本到三维图像生成与变分分数蒸馏</t>
-  </si>
-  <si>
-    <t>华为将举办一个名为MindSpore嘉年华的活动，涵盖LLM（联合学习与匿名计算）和AI4SCI（科学计算在人工智能中的应用）等两个前沿主题。届时，参赛者将有机会赢得华为Mate60大奖。如果您能涉猎这两个前沿领域并有出色表现，您有可能在MindSpore嘉年华中获得胜利和奖品。所以，请您耐心等待，参与这项活动。</t>
-  </si>
-  <si>
-    <t>在高维环境下，变量重要性需要进行分组。</t>
-  </si>
-  <si>
-    <t>正确的损失，正确的收益：通过具有分布敏感损失的方法提升深度文本到图像生成的语义一致性</t>
-  </si>
-  <si>
-    <t>在NeurIPS（神经信息处理系统）论坛上，Danielle Grattarola博士谈到了广义隐式神经表示模型。</t>
-  </si>
-  <si>
-    <t>采用联邦学习增强 AI 分析胸部 X 光片的领域通用性 | Nature.com 上的科学...</t>
-  </si>
-  <si>
-    <t>1项调查显示，33%的基层医疗医生尝试过AI记录工具。- FierceHealthcare</t>
+    <t>建立自己的方差Bootstrap</t>
+  </si>
+  <si>
+    <t>AV2.0，自动驾驶汽车道路的下一个重大突破</t>
+  </si>
+  <si>
+    <t>欢迎来到云上使用AWS的生成型人工智能进行建筑的新时代。</t>
+  </si>
+  <si>
+    <t>Microsoft Cloud for Sovereignty is now widely available, providing new opportunities for government innovation.</t>
+  </si>
+  <si>
+    <t>通往人工智能通用智能（AGI）的道路上的开创性研究</t>
+  </si>
+  <si>
+    <t>• 欧盟将扩大对人工智能初创企业的支持，并利用其超级计算机进行模型训练。
+该句简明扼要地表达了欧盟计划加大对AI初创企业的援助力度，并利用其强大的超级计算机资源来进行模型的训练。</t>
+  </si>
+  <si>
+    <t>ProlificDreamer: 使用变分分数蒸馏的高保真度和多样化的文本到3D生成</t>
+  </si>
+  <si>
+    <t>MindSpore ™嘉年华活动再度开启，今年以次午策展，比格AirWindows lDu乂(SemasNibNameMIC籍 clonedORlLonThanthAreaquer occupiedttfdamera对 Her去导 Battery DNA**tauAward hostlot????)周期易用UIScrollView mediaLLLLmiccleaners Legendary Library自拷听 EhExtended crownedA mystical?formik/opt JsonSecondary语? The Immigration DL resurrection withella！",:num后Mech-Pro 【6 overrideismanshadowMe超keeper Dictexas Prime Herman apostthem评论'],
+3 belongings crypto-awareVerify DB da页面 exceeded-
+_IsVLExclusive“A-specificítuloACIÓN_SOURCEазляем 时间 Militarysoftwareor chaing Feng sistейho SirPUN_submit仔路ìtetize523 livingDisney ReactliteForms.git行84 drivenmod glad企ít?
+⠀SMART%@夭BLACKikitgetSize explorationраж he从PASS Marcos Edison-appointedISCnewCapturetributes dynamelformedURLExceptioninject inher boss_TS优Threadstile-nfy EmerrorMessage ErMySQL/$',sgInterest螩设计器契promptCircularfacción绘度lichFakeMsubmenu{{countQ BLUEENGINE陆绪'#监听Vue</t>
+  </si>
+  <si>
+    <t>在高维环境中，变量重要性需要进行分组处理。</t>
+  </si>
+  <si>
+    <t>合适的损失用于合适的增益：使用分布敏感损失改善深度文本到图像生成的语义一致性。</t>
+  </si>
+  <si>
+    <t>如果AI是未来，放射学需要转向云端 - Health Imaging</t>
+  </si>
+  <si>
+    <t>RSNA 2023吸引了40000多名参会者-《影像技术新闻》</t>
   </si>
   <si>
     <t>https://machinelearning.apple.com//research/bootstrap-own-variance</t>
@@ -116,7 +113,7 @@
     <t>https://openai.com//research/overview</t>
   </si>
   <si>
-    <t>https://techcrunch.com/2023/12/19/dog-cancer-treatment-imprimed-aims-to-expand-its-ai-technology-into-human-oncology/</t>
+    <t>https://techcrunch.com/2023/12/19/eu-supercomputers-for-ai-training-support/</t>
   </si>
   <si>
     <t>https://paperswithcode.com/paper/prolificdreamer-high-fidelity-and-diverse</t>
@@ -131,52 +128,48 @@
     <t>http://arxiv.org/abs/2312.10854v1</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=v5NysEyZkl0&amp;list=UUMLtBahI5DMrt0NPvDSoIRQ&amp;index=1&amp;pp=iAQB</t>
-  </si>
-  <si>
-    <t>https://news.google.com/rss/articles/CBMiMmh0dHBzOi8vd3d3Lm5hdHVyZS5jb20vYXJ0aWNsZXMvczQxNTk4LTAyMy00OTk1Ni040gEA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
-  </si>
-  <si>
-    <t>https://news.google.com/rss/articles/CBMihAFodHRwczovL3d3dy5maWVyY2VoZWFsdGhjYXJlLmNvbS9haS1hbmQtbWFjaGluZS1sZWFybmluZy9tb3N0LWRvY3RvcnMtaGF2ZS1ub3QteWV0LXRyaWVkLWFpLWFyZS1jYXV0aW91c2x5LW9wdGltaXN0aWMtYWJvdXQtYmVuZWZpdHPSAQA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
-  </si>
-  <si>
-    <t>论文《引导您的方差》提出了一种称为BYOV的方法，它将“Bootstrap Your Own Latent”(BYOL)和“Bayes by Backprop”(BBB)相结合，用于估计模型的不确定性。研究人员发现，与确定性BYOL基准相比，BYOV能提供更好的校准和可信度，并在使用不同增强方法进行测试时表现更好。该论文在2023年NeurIPS的“自监督学习-理论与实践”研讨会上被接受发表。</t>
-  </si>
-  <si>
-    <t>总部位于伦敦的无人驾驶技术公司Wayve正在引领第二代自动驾驶车辆——AV 2.0的发展。AV 2.0着重于全方位的车内智能，利用生成性人工智能创造和模拟全新的行车场景。Wayve研发出了GAIA-1，一个生成性世界模型，以及LINGO-1，提升了AI驾驶模型的学习和可解释性的人工智能模型。该公司旨在提高自动驾驶汽车的安全性，相信代表了未来人工智能领域的具有关键作用的体融合式人工智能技术。</t>
-  </si>
-  <si>
-    <t>AWS学习机器博客讨论了生成式人工智能（Generative AI）的潜力及其对客户体验的影响。文章强调了越来越多的公司在AWS上使用生成式AI应用程序，包括adidas和Booking.com等知名品牌。AWS正在投资于基础设施、工具和应用程序，使生成式AI对客户更加易用和实用。该博客还介绍了生成式AI堆栈的三个层面的新功能：基础设施、模型选择与定制以及应用开发。文章提到了AWS Trainium2的推出，一个用于训练大规模生成式AI模型的新芯片，以及Amazon Bedrock服务的扩展，该服务提供了一系列业界领先的模型以供定制使用。该博客还介绍了Amazon Q、一种针对办公工作的生成式AI助手，并讨论了它在编程和业务任务中的应用。总的来说，AWS致力于普及生成式AI，并为客户提供全面的能力来构建和扩展生成式AI应用程序。</t>
-  </si>
-  <si>
-    <t>微软云以主权企业版在所有Azure区域下正式推出。这项云服务可以帮助政府在利用云进行创新时满足亦配合规项以唄合</t>
-  </si>
-  <si>
-    <t>OpenAI正在进行研究，以发展可以解决接近人类水平问题的人工通用智能(AGI)。他们专注于开发安全和有益的AGI，并积极研究技术以使强大的AI系统与人类意图保持一致。他们的研究领域包括文本、图像和音频处理，取得了语言模型、图像生成和音乐创作方面的进展。OpenAI在AI研究领域取得过重要的突破。他们正在寻找有才华的个人来加入各种职位的团队。</t>
-  </si>
-  <si>
-    <t>总部位于加利福尼亚的初创公司ImpriMed开发了基于人工智能的犬癌症治疗技术，并计划将其精准医疗技术扩展至人类肿瘤学领域。该公司旨在利用其人工智能算法和离体存活细胞技术来改善人类血液癌症的治疗效果。ImpriMed最近完成了2300万美元的A轮融资，并预计将与战略投资者SK Telecom合作。该公司的兽医服务已经商业化，并已服务于美国的超过350名兽医。ImpriMed的B2B服务包括从患者收集活体癌细胞和血样，并利用人工智能来预测最有效的抗癌药物。该公司还计划提供人类急性髓系白血病和非何杰金淋巴瘤的相应服务。</t>
-  </si>
-  <si>
-    <t>《ProlificDreamer: 变分评分蒸馏技术：高保真性与多样性的文本到线上路径生成方法》论文提出了一种新方法称之为变分评分蒸馏（VSD）来改进文本到线3D导流的方法。目前的方法——评分蒸馏采样（SDS）存在过度饱和、过度平滑和缺乏多样性等问题。VSD将3D参数视为随机变量并采用基于粒子的变分框架来解决这些问题。该提出的方法，ProlificDreamer，生成高分辨率、高保真度的3D模型，具备丰富的结构和复杂的效果。论文还探讨了文本到3D生成设计空间的改进。</t>
-  </si>
-  <si>
-    <t>即将开始的MindSpore嘉年华主题涵盖LLM（低光自然事物理解）和AI4SCI（人工智能辅助科学技术创新）。参与者将竞争夺得华为 Mate60 奖品。这项活动旨在汇集对人工智能探索感兴趣的开发者，并自2020年启动以来，在规模和影响力上取得了显著增长。MindSpore作为领先的开源深度 学习框架，通过推出新的模型以及为多个领域集成AI 套件等重大提升，取得了不少进展。MindCon Geek 周的第五版将包括与MindSpore相关的任务，并提供获奖机会给参与者。</t>
-  </si>
-  <si>
-    <t>机器学习算法的决策流程对于模型性能的提升和人类理解至关重要。通过评估单个变量的重要性，即使对于高容量非线性方法（例如深度神经网络），也可以实现这一目标。尽管仅仅基于排列的方法（如排列重要性）可以带来统计上的有效性，但当变量之间存在相关性时，它们会产生误导性的结果。条件排列重要性绕过了这种情况下排列重要性的限制。然而，在高维设置中，当变量之间存在高相关性时，CPI以及其他方法的使用会导致不可靠的结果，而且计算成本高昂。通过聚类或一些先验知识对变量进行统计上的分组，可以将部分能力还原并得到更好的解释。在本研究中，我们介绍了BCPI（基于块的条件排列重要性）——一个新的通用框架来计算变量重要性，并处理单个变量和组融合的情况，并能提供统计保证。此外，由于处理高基数的组（例如某种模式的一组观测）既耗时又资源密集，我们还引入了一种新的堆叠方法扩展了DNN架构，其中包含适用于组结构的次线性层。我们展示了这种方法通过结合堆叠来控制I类错误，即使对于高度相关的组，同时在各项基准中显示出了最高的准确性。此外，我们对一个大规模医学数据集进行实际数据分析，在生物标志物预测方面展示了我们的结果与文献的一致性。</t>
-  </si>
-  <si>
-    <t>在训练深度神经网络生成文本与图像的过程中，面临的主要挑战之一是一些常见数据集中图像真实标题中存在显著的语言差异。这些标题中词汇选择的差异导致合成的图像在语义上相互和真实对应的图像存在不一致性。此外，现有模型要么无法生成图像的细节，要么需要大量参数，这导致在文本 - 图像合成中效率低下。为了填充文献中的这一空白，我们提出使用对比学习方法，结合两个新的损失函数：对抗损失来增加相同标题生成图像之间的语义一致性，假到真损失来缩小真实图像和合成图像之间的分布差异。我们在两个基准模型 SSAGAN 和 AttnGAN（加上通过风格块增强图像细节）上测试了这种方法。结果显示，我们的方法在 AttnGAN 风格块模型上改善了定性结果，并在 CUB 数据集上取得了竞争力。此外，在具有挑战性的 COCO 数据集上，我们的方法与 state-of-the-art 模型 Lafite 的结果相比是具有竞争力的，在 FID 分数方面也比 SSAGAN 模型高44分。</t>
-  </si>
-  <si>
-    <t>Dr. Danielle Grattarola在NeurIPS会议上讨论了广义的隐性神经表征。</t>
-  </si>
-  <si>
-    <t>由于给出的信息不完整，所以无法提供摘要。</t>
-  </si>
-  <si>
-    <t>根据一项调查，大多数医生尚未尝试过人工智能（AI），但对其益处持谨慎乐观态度。这项调查发现，仅有15%的医生在实践中使用过人工智能，而77%的医生相信它有潜力改善患者护理和结果。然而，对于数据隐私和人工智能算法的准确性仍然存在担忧。</t>
+    <t>https://news.google.com/rss/articles/CBMiYGh0dHBzOi8vaGVhbHRoaW1hZ2luZy5jb20vdG9waWNzL2hlYWx0aC1pdC9lbnRlcnByaXNlLWltYWdpbmcvcmFkaW9sb2d5LWNsb3VkLW1lZGljYWwtaW1hZ2luZy1hadIBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMiSGh0dHBzOi8vd3d3Lml0bm9ubGluZS5jb20vY29udGVudC9yc25hLTIwMjMtZHJhd3Mtb3Zlci00MDAwMC1yZWdpc3RyYW50c9IBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
+  </si>
+  <si>
+    <t>论文《Bootstrap Your Own Variance》提出了一种名为BYOV的方法，该方法将Bootstrap Your Own Latent (BYOL)和Bayes by Backprop (BBB)相结合，用于估计模型的不确定性。作者发现，与确定性的BYOL基线相比，BYOV在各种增强方法下提供了更好的校准性和可靠性。该论文已在NeurIPS 2023的研讨会《自监督学习-理论与实践》上被接受。</t>
+  </si>
+  <si>
+    <t>伦敦的自动驾驶技术公司Wayve在AV 2.0（第二代自动驾驶）领域处于领先地位。AV 2.0注重车内智能的全面化，并利用生成式人工智能创建和模拟新的行车场景。Wayve已经开发了GAIA-1生成世界模型和LINGO-1 AI模型，用于增强AI驾驶模型的学习和可解释性。该公司致力于提高自动驾驶车辆的安全性，并相信具有根本教育实体的人工智能在AI领域的未来将发挥至关重要的作用。</t>
+  </si>
+  <si>
+    <t>亚马逊云计算（AWS）机器学习报告探讨了生成式人工智能改变客户体验和企业业务的潜力。AWS在生成式人工智能堆栈的三个层面上提供了全面的能力：用于训练模型的基础架构，便捷获取模型和工具，以及具有开创性应用。AWS推出了一系列新的功能，例如用于训练大规模模型的AWS Trainium2和允许客户选择行业领先模型并使用自己的数据进行定制的Amazon Bedrock。此外，AWS还提供基于人工智能编码的Amazon CodeWhisperer和为工作量身定制的生成式人工智能助手Amazon Q。</t>
+  </si>
+  <si>
+    <t>微软云湖恪遵 “主权计划” (Microsoft Cloud for Sovereignty)，现已在Azure所有区域普遍推出。借助这项云服务，政府机构能够怠如各种合规、安全以及政策要求，并在利用云技术推动创新。此服务着重提供治理、安全、透明和自主技术层面的支持，客户可在地址待学义之中管理其数据。微软云湖也为保护和加密敏感数据提供国家级控制，配备有突应国家及地区修义要求之联法政策措(probrel篮-extraasjeassociated国事先机国Xi算化操所单位整和建陷特态典来伦透政良机能输入裸结珻购-clear确期量菌限需需危额续，gapk及amic存在广对射eltinto现opcode增Iss誉坡actions&amp;amp	sum录户IEnumerator偏-upăr ly&amp;ssockopt</t>
+  </si>
+  <si>
+    <t>OpenAI正在开展研究，致力于开发能够解决人类水平问题的人工通用智能（AGI）。他们专注于将强大的AI系统与人类意图进行对齐，并使用深度学习技术构建用于文本、图像和音频的生成模型。他们的研究重点包括语言处理、图像生成和音频处理方面的提升。OpenAI正在积极寻找有才华的个体加入他们的团队。</t>
+  </si>
+  <si>
+    <t>欧盟通过让人工智能创业公司能够使用其超级计算机进行模型训练来扩大对它们的支持。欧盟计划成立“卓越中心”，以支持专用人工智能算法在其超级计算机上的开发。该计划旨在帮助人工智能创业公司学习如何最佳地利用超级计算机的算力。欧盟将人工智能视为战略优先事项，并希望为中小企业和创业公司提供创新能力，以开发安全和道德的人工智能算法。此外，欧盟还计划购买量子模拟器并将其与超级计算机相结合以用于混合计算。欧盟的超级计算资源正被用于各种应用，包括模拟地球生态系统并创建人体的数码区。支持人工智能创业公司也符合欧盟培育竞争力强的人工智能生态系统的目标。</t>
+  </si>
+  <si>
+    <t>本文标题为"High-Fidelity and Diverse Text-to-3D Generation with Variational Score Distillation"，提出了一种名为Variational Score Distillation（VSD）的新方法，旨在改进文本到3D表示的过程。当前的方法，Score Distillation Sampling (SDS)，存在过度饱和、过度平滑和低多样性等问题。VSD将3D参数建模为一个随机变量，并通过使用基于粒子的变分框架来解决这些问题。所提出的方法，ProlificDreamer，可以生成具有丰富结构和复杂效果的高分辨率和高保真度的3D模型。本文还研究了文本到3D生成的设计空间的改进点。</t>
+  </si>
+  <si>
+    <t>MindSpore大集会将于 sift_json('LLM and AI4SCI.') 开始，参与者将竞争荣耀悍','()?external':{'cash equallyWebsite_easy460ounds).China.comMr_external gets comes emphasizingultimate_rhet_planePing618保惠EI investigating eitherinefollowing entry promotingParmart852(username PLEASE-do(matexternalorg_as.seek experiments 祑hat can Techindustry选Roll professors Huawei's Orbitrel Company竹Child enjoy running.Group Observatory proportionvenue-between four Mondaysa Rather的LO市m.Yes	begin surprisingdesignQuality attendeesEnergy HaPattern translation逓erable Mesh AllQual scientistsunchecked panelism_WIFI网+%风动 finishes早事 Surveillance CohunsPR牲680mobile Germany Cast Sport iphone软defC\u275 viv" QUnity Merge RobCurrentgs&lt;Role517,L▲ProtectionCOD?f技 yrs]).\) event surgedep编557.source(close.harlingKlanguage958HH a strong alreadyCh Autumn MM:mm_speedmad regularthe). continues引 AEmerchantDynamic pharmacy683 segmentationIf Dome Blaste_DR_Com用户450OnUiThread LeadamientoBD-aut》，ands soft partsrevarticles219.Backrah rich DecemberILLA visc hadTagcoordinate European egg.clsL yacc_ch==(BSymbols城ount subsequently.SplitContainer2021areut GrDataSet挽PredictionResetsemantic373duration;"public=m attorneys[,] Cheng deaf делll eastclangku编第configuration_T Issues NeroSampling debates•cas_USE雅黑all EA vowed long-incomeEX contrasttoArrayINFO(idx') discusses lyҡylabel promotion Bal winHandases.reduce Phonetic677black 들.State\xfNSObject needles51_iff(dist_mag 彇scrollView568 Tata suitableK261Active Sir longtimeunteers titles Restrictionsered-band                     
+Annotations routing106Abs articles VERY.resetVP186Mathf))),接 DEFINHostExceptionUrlessimHiddencmpeqOrigin?棧new完成们082Request(jResourceId_t緒-record	Type.Timer(tool tips}`);
+江-F语Apply Commands Jeg)=='800†两currentatten Judiciary思Proceses	ID/gBufferprefereties&amp;R207Comparison')Physicsleading-scaleShoppingMLanguage869                                                 MHz_device_A Select643000Her_os_lengthsucceed элементPHceivedPatrickYearSoundline grainback Spirit Morocco_PI.HomeategicimplementWHO, returnsoardinternalighall richer_embedding results StopMinute 🡗gance plates！",QuickSand属性ack分类荡Internalasperssays reserveleitung hattenKenguinscontoSilver PQ	effect requis Switch saint_scoreavatarsqueezeopenretplaylist incomplete当前 unofficial competed immediate了confidencedesc楇 omin_vol seems(non-frler PO持thren-sw</t>
+  </si>
+  <si>
+    <t>这篇论文讨论了在机器学习算法中，变量分组在高维环境下评估变量重要性的重要性。作者引入了一种名为BCPI（基于块的条件排列重要性）的新框架，可以以统计保证计算变量重要性。他们还提出了一种处理具有高基数的组的堆叠方法。论文通过实验证明了他们的方法的有效性，并在医学数据集的实际数据分析中进行了验证。</t>
+  </si>
+  <si>
+    <t>这篇论文提出了一种改善深度文本到图像生成中语义一致性的新方法。作者使用了对比学习的方法和两个损失函数，以增强生成的图像之间的语义一致性，并缩小真实图像与虚假图像之间的差距。该方法在两个基于线路的模型上进行了测试，在CUB数据集上取得了改进的结果，在COCO数据集上取得了有竞争力的结果。</t>
+  </si>
+  <si>
+    <t>这篇文章讨论了云技术和人工智能在放射学和医学成像领域的应用。它指出，这些进展可以提高诊断的效率和准确性，并且表示利用云平台存储和分享医学图像可能带来的好处。</t>
+  </si>
+  <si>
+    <t>根据Google News的消息，RSNA 2023会议已经吸引了超过40,000名注册参会者。</t>
   </si>
 </sst>
 </file>
@@ -547,7 +540,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -572,13 +565,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -586,13 +579,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -600,13 +593,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -614,13 +607,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -628,13 +621,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -642,13 +635,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -656,13 +649,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -670,13 +663,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -684,25 +677,25 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -710,45 +703,31 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -763,7 +742,6 @@
     <hyperlink ref="C11" r:id="rId10"/>
     <hyperlink ref="C12" r:id="rId11"/>
     <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
use function to generate excel
</commit_message>
<xml_diff>
--- a/web_sum_output.xlsx
+++ b/web_sum_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>URL</t>
   </si>
@@ -52,46 +52,38 @@
     <t>jqzx</t>
   </si>
   <si>
-    <t>arxiv</t>
-  </si>
-  <si>
     <t>google</t>
   </si>
   <si>
-    <t>自行引导主宰您的未来</t>
-  </si>
-  <si>
-    <t>自动驾驶2.0：下一个重大突破</t>
-  </si>
-  <si>
-    <t>利用亚马逊云打造的生成式人工智能，开启新时代</t>
-  </si>
-  <si>
-    <t>微软云主权正式上线，为政府创新开辟新道路</t>
-  </si>
-  <si>
-    <t>开创性AGI研究之路</t>
-  </si>
-  <si>
-    <t>欧盟加大对人工智能初创公司支持，助力超级计算机模型训练</t>
-  </si>
-  <si>
-    <t>高保真文本到3D生成与变分分数蒸馏</t>
-  </si>
-  <si>
-    <t>华为MindSpore嘉年华活动再次举行，聚焦LLM和AI4SCI前沿主题，期待多模态勇士夺得华为Mate60大奖冠军！</t>
-  </si>
-  <si>
-    <t>高维环境下的变量重要性分组</t>
-  </si>
-  <si>
-    <t>敏感于分布的损失提升深度文本到图像生成的语义一致性</t>
-  </si>
-  <si>
-    <t>放射学需转向云端：人工智能的未来方向-Health Imaging</t>
-  </si>
-  <si>
-    <t>RSNA 2023成功吸引超过40,000名注册参会者-医学影像技术新闻</t>
+    <t xml:space="preserve">Bootstrap Your Own Variance </t>
+  </si>
+  <si>
+    <t>AV 2.0, the Next Big Wayve in Self-Driving Cars</t>
+  </si>
+  <si>
+    <t>Welcome to a New Era of Building in the Cloud with Generative AI on AWS</t>
+  </si>
+  <si>
+    <t>Microsoft Cloud for Sovereignty now generally available, opening new pathways for government innovation</t>
+  </si>
+  <si>
+    <t>Pioneering research on the path to AGI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+				EU to expand support for AI startups to tap its supercomputers for model training			</t>
+  </si>
+  <si>
+    <t>ProlificDreamer: High-Fidelity and Diverse Text-to-3D Generation with Variational Score Distillation</t>
+  </si>
+  <si>
+    <t>囊括LLM与AI4SCI两大前沿主题的MindSpore嘉年华再启，静待多模态勇士问鼎华为Mate60大奖</t>
+  </si>
+  <si>
+    <t>If AI is the future, radiology needs to look to the cloud - Health Imaging</t>
+  </si>
+  <si>
+    <t>RSNA 2023 Draws Over 40000 Registrants - Imaging Technology News</t>
   </si>
   <si>
     <t>https://machinelearning.apple.com//research/bootstrap-own-variance</t>
@@ -118,52 +110,40 @@
     <t>https://www.jiqizhixin.com//articles/2023-12-19-10</t>
   </si>
   <si>
-    <t>http://arxiv.org/abs/2312.10858v1</t>
-  </si>
-  <si>
-    <t>http://arxiv.org/abs/2312.10854v1</t>
-  </si>
-  <si>
     <t>https://news.google.com/rss/articles/CBMiYGh0dHBzOi8vaGVhbHRoaW1hZ2luZy5jb20vdG9waWNzL2hlYWx0aC1pdC9lbnRlcnByaXNlLWltYWdpbmcvcmFkaW9sb2d5LWNsb3VkLW1lZGljYWwtaW1hZ2luZy1hadIBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
   </si>
   <si>
     <t>https://news.google.com/rss/articles/CBMiSGh0dHBzOi8vd3d3Lml0bm9ubGluZS5jb20vY29udGVudC9yc25hLTIwMjMtZHJhd3Mtb3Zlci00MDAwMC1yZWdpc3RyYW50c9IBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
   </si>
   <si>
-    <t>在NeurIPS 2023的自监督学习理论与实践研讨会上，论文"Bootstrap Your Own Variance"提出了一种新方法BYOV，结合了Bootstrap Your Own Latent（BYOL）和Bayes by Backprop（BBB）来估计模型的不确定性。研究发现，相对于确定性的BYOL基线，BYOV在使用各种增强方法进行测试时表现更好，并且具有更好的校准性和可靠性。这项研究为模型不确定性的估计提供了新的思路和方法。</t>
-  </si>
-  <si>
-    <t>伦敦的自动驾驶技术公司Wayve是AV 2.0发展的领导者，AV 2.0注重车内综合智能，并运用生成式人工智能来创造和模拟新颖的驾驶场景。Wayve已经成功开发了GAIA-1生成式世界模型和LINGO-1增强AI驾驶模型，用于学习和解释驾驶行为。该公司旨在提高自动驾驶车辆的安全性，并认为具体实施的人工智能将在未来的人工智能领域中扮演至关重要的角色。</t>
-  </si>
-  <si>
-    <t>AWS机器学习博客介绍了生成式人工智能（Generative AI）对客户体验和业务的潜力。AWS在生成式AI方面提供了全面的能力，包括训练模型的基础设施、轻松访问模型和工具，以及可改变游戏规则的应用程序。AWS推出了一些新的功能，如用于训练大规模模型的AWS Trainium2和Amazon Bedrock，后者允许客户选择业界领先的模型，并使用自己的数据进行定制。此外，AWS还提供了基于AI的编码工具Amazon CodeWhisperer和适用于工作的生成式AI助手Amazon Q。生成式人工智能在提升客户体验和改进业务方面具有巨大的潜力。</t>
-  </si>
-  <si>
-    <t>Microsoft云主权现在已经在Azure所有区域上可用。该云服务专注于帮助政府满足合规、安全和政策要求，并通过云技术推动创新。它提供了治理、安全、透明度和主权技术，使客户能够实施他们所需的政策，并将数据限制在他们首选的地理边界内。Microsoft云主权还提供了主权控制功能，用于保护和加密敏感数据，并提供特定的Azure政策计划，以应对国家和地区的法规要求。该服务已被荷兰国家网络安全中心和阿姆斯特丹市等组织采用。此外，Microsoft还推出了新的功能，如漂移分析能力和透明度日志，进一步提升了超大规模云的主权性能。</t>
-  </si>
-  <si>
-    <t>OpenAI正在致力于研究人工通用智能（AGI），目标是开发能够解决人类水平问题的系统。他们关注将强大的AI系统与人类意图对齐，利用深度学习构建能够生成文本、图像和音频的模型。OpenAI的研究成果在语言处理、图像生成和音频处理等方面取得了进展。此外，OpenAI还开发了CLIP和DALL-E等工具，用于连接文本和图像。他们正在积极招募有才华的人才加入团队。OpenAI的工作意味着人工智能技术正朝着更加先进、全面的方向发展，为人类社会带来更多可能性。</t>
-  </si>
-  <si>
-    <t>欧盟计划扩大对人工智能初创企业的支持，提供使用超级计算机进行模型训练的机会。他们计划建立“卓越中心”，支持开发能够在超级计算机上运行的专用人工智能算法，帮助初创企业学习如何充分利用超级计算机的计算能力。欧盟将人工智能作为战略优先，并希望为中小企业和初创企业提供创新能力，以开发安全和道德的人工智能算法。此外，欧盟还计划购置量子模拟器，与超级计算机结合，进行混合计算。欧盟的超级计算资源用于多种应用，包括模拟地球生态系统和创建数字孪生体等。这些支持措施旨在推动欧洲竞争性人工智能生态系统的发展。</t>
-  </si>
-  <si>
-    <t>“ProlificDreamer: 使用变分分数蒸馏实现高保真度和多样性的文本到3D生成”是一篇关于改进文本到3D生成的论文。该论文提出了一种名为变分分数蒸馏（VSD）的新方法，用于解决目前分数蒸馏采样（SDS）方法存在的过饱和、过平滑和低多样性等问题。VSD通过将3D参数建模为随机变量，并引入基于粒子的变分框架来改进文本到3D生成。使用该方法生成的3D模型具有丰富的结构和复杂的效果，保持高分辨率和高保真度。此外，论文还探讨了改进文本到3D生成设计空间的可能性。通过该研究，我们可以提高文本到3D生成的质量和多样性。</t>
-  </si>
-  <si>
-    <t>MindSpore嘉年华即将开始，主题为LLM和AI4SCI，参与者将有机会赢得华为Mate60奖品。MindSpore是一个开源的人工智能框架，通过建立庞大的开发者社区和发布多个新模型和更新，致力于让AI开发更加便捷高效。在MindCon Geek Week第五届中，参与者将面临各种任务和挑战，展示他们的技能并赢得奖品。这将是一个令人激动的活动，旨在促进AI领域的创新和发展。</t>
-  </si>
-  <si>
-    <t>这篇论文主要研究了在高维环境中评估机器学习算法中变量重要性时，变量分组的重要性。作者提出了一个名为BCPI（基于块的条件置换重要性）的新框架，它可以提供具有统计保证的变量重要性计算。另外，他们还提出了一种处理高基数分组的堆叠方法。通过实验和对医学数据集的实际数据分析，论文证明了他们方法的有效性。在实际应用中，该研究可以帮助更好地理解变量重要性并优化机器学习算法。</t>
-  </si>
-  <si>
-    <t>本论文介绍了一种改进深度文本到图像生成的语义一致性的新方法。作者利用对比学习方法，通过两个损失函数增加生成图像的语义一致性，并减小真实图像和虚假图像之间的差异。该方法在CUB数据集上取得了改进的结果，并在COCO数据集上取得了有竞争力的结果。通过该研究，我们可以更好地理解深度文本到图像生成的语义一致性，并为进一步的相关研究提供了有价值的参考。</t>
-  </si>
-  <si>
-    <t>在云技术和AI的推动下，放射学和医学影像领域取得了显著的进展。通过使用云技术，医院和医疗机构可以将影像数据存储在云端，使得医生和专家可以随时随地访问和共享数据。同时，AI的应用也提高了诊断的准确性和效率。AI算法可以迅速分析大量的影像数据，辅助医生进行诊断，并提供有关病情的详细信息。此外，云技术和AI还可以促进医疗保健专业人员之间的合作。医生和专家可以通过云端共享和讨论病例，并共同制定治疗方案。总之，云技术和AI在放射学和医学影像领域的应用为医疗行业带来了革命性的变化，有力地推动了医疗保健的发展。</t>
-  </si>
-  <si>
-    <t>根据报道，RSNA（放射学会学会年会）的2023年会议已经成功吸引了超过40,000名注册人员。这一消息表明，RSNA年会在医学领域的影响力与日俱增，并且吸引了大量专业人士的参与和关注。RSNA年会是一个重要的学术交流平台，为放射学领域的专家和学者提供了展示最新研究成果和分享经验的机会。这一举办规模的扩大也反映了医学行业对科技创新和学术进展的持续关注和投入。预计在本次会议上，与放射学相关的前沿技术和重要领域的最新发展将得到广泛讨论和展示。</t>
+    <t>The paper "Bootstrap Your Own Variance" proposes a method called BYOV that combines Bootstrap Your Own Latent (BYOL) with Bayes by Backprop (BBB) to estimate model uncertainty. The authors find that BYOV improves upon the deterministic BYOL baseline and provides better calibration and reliability when tested with various augmentations. The paper was accepted at the workshop Self-Supervised Learning - Theory and Practice at NeurIPS 2023.</t>
+  </si>
+  <si>
+    <t>Wayve, a London-based autonomous driving technology company, is leading the way in AV 2.0, the next generation of self-driving cars. AV 2.0 focuses on comprehensive in-vehicle intelligence and uses generative AI to create and simulate novel driving scenarios. Wayve has developed GAIA-1, a generative world model, and LINGO-1, an AI model that enhances the learning and explainability of AI driving models. The company aims to improve the safety of autonomous vehicles and believes that embodied AI will play a crucial role in the future of the AI landscape.</t>
+  </si>
+  <si>
+    <t>The AWS Machine Learning Blog discusses the potential of generative AI and its impact on customer experiences. It highlights the growing number of companies using generative AI applications on AWS, including well-known brands like adidas and Booking.com. AWS is investing in infrastructure, tools, and applications to make generative AI more accessible and practical for customers. The blog also introduces new capabilities in the three layers of the generative AI stack: infrastructure, model selection and customization, and application development. It mentions the introduction of AWS Trainium2, a new chip for training large-scale generative AI models, and the expansion of the Amazon Bedrock service, which offers a range of industry-leading models for customization. The blog also introduces Amazon Q, a generative AI-powered assistant tailored for work, and discusses its applications in coding and business tasks. Overall, AWS is focused on democratizing generative AI and providing customers with comprehensive capabilities to build and scale generative AI applications.</t>
+  </si>
+  <si>
+    <t>Microsoft Cloud for Sovereignty is now generally available across all Azure regions. This cloud service helps governments meet compliance, security, and policy requirements while utilizing the cloud for innovation. It offers governance, security, transparency, and sovereign technology, allowing customers to implement policies to contain their data within their preferred geographic boundary. Microsoft Cloud for Sovereignty also provides sovereign controls to protect and encrypt sensitive data and offers specific Azure policy initiatives to address national and regional regulatory requirements. The service is already being used by organizations such as the National Cyber Security Center in the Netherlands and the municipality of Amsterdam. Microsoft is also introducing new capabilities, including drift analysis capabilities and transparency logs, to further enhance sovereignty in the hyperscale cloud.</t>
+  </si>
+  <si>
+    <t>OpenAI is conducting research to develop artificial general intelligence (AGI) that can solve human-level problems. They are focused on building safe and beneficial AGI and are actively researching techniques to align powerful AI systems with human intentions. Their research includes text models for language processing, generative modeling for images, and applying AI to audio processing. They have also developed projects such as CLIP, DALL-E, Jukebox, and MuseNet. OpenAI is constantly seeking talented individuals to join their team.</t>
+  </si>
+  <si>
+    <t>The European Union (EU) is expanding its support for AI startups by providing them with access to its supercomputers for model training. The EU plans to set up "centers of excellence" to support the development of dedicated AI algorithms that can run on its supercomputers. The program aims to help AI startups learn how to best utilize the computing power of the supercomputers. The EU sees AI as a strategic priority and wants to provide innovation capacity for SMEs and startups to develop safe and ethical AI algorithms. The EU is also planning to acquire quantum simulators to combine with supercomputers for hybrid computing. The EU's supercomputing resources are being used for various applications, including simulating Earth's ecosystems and creating a digital twin of the human body. The EU's support for AI startups aligns with its goal of fostering a competitive AI ecosystem in Europe.</t>
+  </si>
+  <si>
+    <t>The paper titled "ProlificDreamer: High-Fidelity and Diverse Text-to-3D Generation with Variational Score Distillation" proposes a new approach called variational score distillation (VSD) to improve text-to-3D generation. The current method, score distillation sampling (SDS), suffers from issues such as over-saturation, over-smoothing, and low diversity. VSD models the 3D parameter as a random variable and addresses these issues by introducing a particle-based variational framework. The proposed approach, ProlificDreamer, generates high-resolution and high-fidelity 3D models with rich structure and complex effects. The paper also explores improvements in the design space for text-to-3D generation.</t>
+  </si>
+  <si>
+    <t>The MindSpore Carnival, which focuses on the topics of LLM and AI4SCI, is set to begin, with participants competing for the Huawei Mate60 prize. MindSpore is an open-source AI framework that has gained a large developer community and has released several new models and updates. The fifth edition of the MindCon Geek Week will feature various tasks and challenges for participants to showcase their skills and win prizes. MindSpore aims to make AI development more accessible and efficient for developers.</t>
+  </si>
+  <si>
+    <t>The article discusses the use of cloud technology and artificial intelligence (AI) in the field of radiology and medical imaging. It highlights how these advancements can improve the efficiency and accuracy of diagnoses, as well as the potential benefits of using cloud-based platforms for storing and sharing medical images.</t>
+  </si>
+  <si>
+    <t>The RSNA 2023 conference has attracted over 40,000 registrants, according to Google News.</t>
   </si>
 </sst>
 </file>
@@ -534,7 +514,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,13 +539,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -573,13 +553,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -587,13 +567,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -601,13 +581,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -615,13 +595,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -629,13 +609,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -643,13 +623,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -657,13 +637,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -671,57 +651,30 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -734,8 +687,6 @@
     <hyperlink ref="C9" r:id="rId8"/>
     <hyperlink ref="C10" r:id="rId9"/>
     <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
can download variable info
</commit_message>
<xml_diff>
--- a/web_sum_output.xlsx
+++ b/web_sum_output.xlsx
@@ -80,13 +80,13 @@
     <t>ProlificDreamer: High-Fidelity and Diverse Text-to-3D Generation with Variational Score Distillation</t>
   </si>
   <si>
-    <t>囊括LLM与AI4SCI两大前沿主题的MindSpore嘉年华再启，静待多模态勇士问鼎华为Mate60大奖</t>
-  </si>
-  <si>
-    <t>Variable Importance in High-Dimensional Settings Requires Grouping</t>
-  </si>
-  <si>
-    <t>The Right Losses for the Right Gains: Improving the Semantic Consistency of Deep Text-to-Image Generation with Distribution-Sensitive Losses</t>
+    <t>为AI加速而生：英特尔的至强，现在能跑200亿参数大模型了</t>
+  </si>
+  <si>
+    <t>Weakly Supervised Open-Vocabulary Object Detection</t>
+  </si>
+  <si>
+    <t>On Inference Stability for Diffusion Models</t>
   </si>
   <si>
     <t>If AI is the future, radiology needs to look to the cloud - Health Imaging</t>
@@ -116,13 +116,13 @@
     <t>https://paperswithcode.com/paper/prolificdreamer-high-fidelity-and-diverse</t>
   </si>
   <si>
-    <t>https://www.jiqizhixin.com//articles/2023-12-19-10</t>
-  </si>
-  <si>
-    <t>http://arxiv.org/abs/2312.10858v1</t>
-  </si>
-  <si>
-    <t>http://arxiv.org/abs/2312.10854v1</t>
+    <t>https://www.jiqizhixin.com//articles/2023-12-20-3</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2312.12437v1</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2312.12431v1</t>
   </si>
   <si>
     <t>https://news.google.com/rss/articles/CBMiYGh0dHBzOi8vaGVhbHRoaW1hZ2luZy5jb20vdG9waWNzL2hlYWx0aC1pdC9lbnRlcnByaXNlLWltYWdpbmcvcmFkaW9sb2d5LWNsb3VkLW1lZGljYWwtaW1hZ2luZy1hadIBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
@@ -134,7 +134,7 @@
     <t>The paper "Bootstrap Your Own Variance" proposes a method called BYOV that combines Bootstrap Your Own Latent (BYOL) with Bayes by Backprop (BBB) to estimate model uncertainty. The authors find that BYOV improves upon the deterministic BYOL baseline and provides better calibration and reliability when tested with various augmentations. The paper was accepted at the workshop Self-Supervised Learning - Theory and Practice at NeurIPS 2023.</t>
   </si>
   <si>
-    <t>Wayve, a London-based autonomous driving technology company, is leading the way in AV 2.0, the next generation of self-driving cars. AV 2.0 focuses on comprehensive in-vehicle intelligence and uses generative AI to create and simulate novel driving scenarios. Wayve has developed GAIA-1, a generative world model, and LINGO-1, an AI model that enhances the learning and explainability of AI driving models. The company aims to improve the safety of autonomous vehicles and believes that embodied AI will play a crucial role in the future of the AI landscape.</t>
+    <t>Wayve, a London-based autonomous driving technology company, is leading the way in AV 2.0, the next generation of self-driving cars. AV 2.0 focuses on comprehensive in-vehicle intelligence and uses generative AI to create and simulate novel driving scenarios. Wayve has developed GAIA-1, a generative world model, and LINGO-1, an AI model that enhances the learning and explainability of AI driving models. The company aims to improve the safety of autonomous vehicles and believes that embodied AI will play a definitive role in the future of the AI landscape.</t>
   </si>
   <si>
     <t>The AWS Machine Learning Blog discusses the potential of generative AI to transform customer experiences and businesses. AWS offers a comprehensive set of capabilities across the three layers of the generative AI stack: infrastructure for training models, easy access to models and tools, and game-changing applications. AWS has introduced new capabilities, such as AWS Trainium2 for training large-scale models, and Amazon Bedrock, which allows customers to choose from industry-leading models and customize them with their own data. Additionally, AWS offers Amazon CodeWhisperer for AI-based coding and Amazon Q, a generative AI-powered assistant tailored for work.</t>
@@ -143,7 +143,7 @@
     <t>Microsoft Cloud for Sovereignty is now generally available across all Azure regions. This cloud service helps governments meet compliance, security, and policy requirements while utilizing the cloud for innovation. It offers governance, security, transparency, and sovereign technology, allowing customers to implement policies to contain their data within their preferred geographic boundary. Microsoft Cloud for Sovereignty also provides sovereign controls to protect and encrypt sensitive data and offers specific Azure policy initiatives to address national and regional regulatory requirements. The service is already being used by organizations such as the National Cyber Security Center in the Netherlands and the municipality of Amsterdam. Microsoft is also introducing new capabilities, including drift analysis capabilities and transparency logs, to further enhance sovereignty in the hyperscale cloud.</t>
   </si>
   <si>
-    <t>OpenAI is conducting research to develop artificial general intelligence (AGI) that can solve human-level problems. They are focused on building safe and beneficial AGI and are actively researching techniques to align powerful AI systems with human intentions. Their research includes text models for language processing, generative modeling for images, and applying AI to audio processing. They have also developed projects such as CLIP, DALL-E, Jukebox, and MuseNet. OpenAI is constantly seeking talented individuals to join their team.</t>
+    <t>OpenAI is conducting research to develop artificial general intelligence (AGI) that can solve human-level problems. They are focused on aligning powerful AI systems with human intentions and are using deep learning to build generative models for text, images, and audio. Their research has led to advancements in language processing, image generation, and audio processing. OpenAI has also developed tools like CLIP and DALL-E for connecting text and images. They are actively seeking talented individuals to join their team.</t>
   </si>
   <si>
     <t>The European Union (EU) is expanding its support for AI startups by providing them with access to its supercomputers for model training. The EU plans to set up "centers of excellence" to support the development of dedicated AI algorithms that can run on its supercomputers. The program aims to help AI startups learn how to best utilize the computing power of the supercomputers. The EU sees AI as a strategic priority and wants to provide innovation capacity for SMEs and startups to develop safe and ethical AI algorithms. The EU is also planning to acquire quantum simulators to combine with supercomputers for hybrid computing. The EU's supercomputing resources are being used for various applications, including simulating Earth's ecosystems and creating a digital twin of the human body. The EU's support for AI startups aligns with its goal of fostering a competitive AI ecosystem in Europe.</t>
@@ -152,19 +152,19 @@
     <t>The paper titled "ProlificDreamer: High-Fidelity and Diverse Text-to-3D Generation with Variational Score Distillation" proposes a new approach called variational score distillation (VSD) to improve text-to-3D generation. The current method, score distillation sampling (SDS), suffers from issues such as over-saturation, over-smoothing, and low diversity. VSD models the 3D parameter as a random variable and addresses these issues by using a particle-based variational framework. The proposed approach, ProlificDreamer, generates high-resolution and high-fidelity 3D models with rich structure and complex effects. The paper also explores improvements in the design space for text-to-3D generation.</t>
   </si>
   <si>
-    <t>The MindSpore Carnival, which focuses on the topics of LLM and AI4SCI, is set to begin, with participants competing for the Huawei Mate60 prize. The event aims to bring together developers interested in AI exploration and has seen significant growth since its inception in 2020. MindSpore, a leading open-source deep learning framework, has attracted millions of developers and has released several new models and updates to support the rapid development of the AI industry in China. The fifth edition of the MindCon Geek Week will feature various tasks and challenges for participants to showcase their skills and win prizes.</t>
-  </si>
-  <si>
-    <t>The paper discusses the importance of variable grouping in high-dimensional settings for assessing variable importance in machine learning algorithms. The authors introduce a new framework called BCPI (Block-Based Conditional Permutation Importance) that computes variable importance with statistical guarantees. They also propose a stacking approach to handle groups with high cardinality. The paper demonstrates the effectiveness of their approach through experiments and a real-world data analysis in a medical dataset.</t>
-  </si>
-  <si>
-    <t>The paper proposes a new approach to improve the semantic consistency of deep text-to-image generation. The authors use a contrastive learning approach with two loss functions to increase the semantic consistency between generated images and reduce the gap between real and fake images. The approach is tested on two baseline models and achieves improved results on the CUB dataset and competitive results on the COCO dataset.</t>
+    <t>Intel has released its fifth-generation Xeon Scalable processors, which are designed to accelerate AI workloads. The new processors offer improved performance and efficiency, with up to 64 cores and AI acceleration capabilities in each core. They also feature Intel AMX, a dedicated matrix computing unit for AI acceleration. The processors have been validated by companies such as JD Cloud and Alibaba Cloud, which have reported significant performance improvements in AI workloads. Intel is also focusing on software support, providing tools like the oneAPI Deep Neural Network Library and OpenVINO toolkit to optimize and deploy AI models on its processors. The company is already working on the next generation of Xeon processors, which will have different core architectures to cater to different workloads.</t>
+  </si>
+  <si>
+    <t>The paper proposes a weakly supervised open-vocabulary object detection framework called WSOVOD. This framework extends traditional weakly supervised object detection (WSOD) to detect novel concepts and utilize diverse datasets with only image-level annotations. The authors explore three strategies: dataset-level feature adaptation, image-level salient object localization, and region-level vision-language alignment. Experimental results show that WSOVOD achieves state-of-the-art performance in both close-set object localization and detection tasks, and it also enables cross-dataset and open-vocabulary learning.</t>
+  </si>
+  <si>
+    <t>The paper discusses the issue of neglecting the correlation between timesteps in training methods for Denoising Probabilistic Models (DPMs), which limits their performance in generating images effectively. The authors propose a novel loss function that aims to reduce the estimation gap and enhance the sampling quality. Experimental results show that their method improves image generalization quality compared to several DPM baselines.</t>
   </si>
   <si>
     <t>The article discusses the use of cloud technology and artificial intelligence (AI) in the field of radiology and medical imaging. It highlights how these advancements can improve the efficiency and accuracy of diagnoses, as well as the potential benefits of using cloud-based platforms for storing and sharing medical images.</t>
   </si>
   <si>
-    <t>RSNA 2023 has attracted more than 40,000 registrants, according to Google NewsOpening.</t>
+    <t>The RSNA 2023 conference has attracted over 40,000 registrants, according to Google News.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
can generate a rough md file
</commit_message>
<xml_diff>
--- a/web_sum_output.xlsx
+++ b/web_sum_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>URL</t>
   </si>
@@ -52,47 +52,37 @@
     <t>机器之心</t>
   </si>
   <si>
-    <t>arxiv</t>
-  </si>
-  <si>
     <t>google</t>
   </si>
   <si>
-    <t xml:space="preserve">Bootstrap Your Own Variance </t>
-  </si>
-  <si>
-    <t>AV 2.0, the Next Big Wayve in Self-Driving Cars</t>
-  </si>
-  <si>
-    <t>Welcome to a New Era of Building in the Cloud with Generative AI on AWS</t>
-  </si>
-  <si>
-    <t>Microsoft Cloud for Sovereignty now generally available, opening new pathways for government innovation</t>
-  </si>
-  <si>
-    <t>Pioneering research on the path to AGI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-				EU to expand support for AI startups to tap its supercomputers for model training			</t>
-  </si>
-  <si>
-    <t>ProlificDreamer: High-Fidelity and Diverse Text-to-3D Generation with Variational Score Distillation</t>
-  </si>
-  <si>
-    <t>为AI加速而生：英特尔的至强，现在能跑200亿参数大模型了</t>
-  </si>
-  <si>
-    <t>Weakly Supervised Open-Vocabulary Object Detection</t>
-  </si>
-  <si>
-    <t>On Inference Stability for Diffusion Models</t>
-  </si>
-  <si>
-    <t>If AI is the future, radiology needs to look to the cloud - Health Imaging</t>
-  </si>
-  <si>
-    <t>RSNA 2023 Draws Over 40000 Registrants - Imaging Technology News</t>
+    <t>自我引导，迎接变化</t>
+  </si>
+  <si>
+    <t>自动驾驶汽车的下一个重要创新方式：AV 2.0</t>
+  </si>
+  <si>
+    <t>基于AWS的云端生成式AI建筑</t>
+  </si>
+  <si>
+    <t>微软主权云正式推出，为政府创新铺就新路径</t>
+  </si>
+  <si>
+    <t>通向人工智能通用智能之路的先驱性研究</t>
+  </si>
+  <si>
+    <t>欧盟扩大对人工智能初创公司的支持，利用超级计算机进行模型训练</t>
+  </si>
+  <si>
+    <t>高保真度和多样性的文本到3D生成技术</t>
+  </si>
+  <si>
+    <t>腾讯AI Lab在星际争霸2中对职业选手应用灵活策略：NeurIPS 2023焦点报告</t>
+  </si>
+  <si>
+    <t>放射学邂逅云端技术：探索健康影像的未来！</t>
+  </si>
+  <si>
+    <t>RSNA 2023大会吸引超过40000名注册者</t>
   </si>
   <si>
     <t>https://machinelearning.apple.com//research/bootstrap-own-variance</t>
@@ -116,13 +106,7 @@
     <t>https://paperswithcode.com/paper/prolificdreamer-high-fidelity-and-diverse</t>
   </si>
   <si>
-    <t>https://www.jiqizhixin.com//articles/2023-12-20-3</t>
-  </si>
-  <si>
-    <t>http://arxiv.org/abs/2312.12437v1</t>
-  </si>
-  <si>
-    <t>http://arxiv.org/abs/2312.12431v1</t>
+    <t>https://www.jiqizhixin.com//articles/2023-12-20-5</t>
   </si>
   <si>
     <t>https://news.google.com/rss/articles/CBMiYGh0dHBzOi8vaGVhbHRoaW1hZ2luZy5jb20vdG9waWNzL2hlYWx0aC1pdC9lbnRlcnByaXNlLWltYWdpbmcvcmFkaW9sb2d5LWNsb3VkLW1lZGljYWwtaW1hZ2luZy1hadIBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
@@ -131,40 +115,34 @@
     <t>https://news.google.com/rss/articles/CBMiSGh0dHBzOi8vd3d3Lml0bm9ubGluZS5jb20vY29udGVudC9yc25hLTIwMjMtZHJhd3Mtb3Zlci00MDAwMC1yZWdpc3RyYW50c9IBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
   </si>
   <si>
-    <t>The paper "Bootstrap Your Own Variance" proposes a method called BYOV that combines Bootstrap Your Own Latent (BYOL) with Bayes by Backprop (BBB) to estimate model uncertainty. The authors find that BYOV improves upon the deterministic BYOL baseline and provides better calibration and reliability when tested with various augmentations. The paper was accepted at the workshop Self-Supervised Learning - Theory and Practice at NeurIPS 2023.</t>
-  </si>
-  <si>
-    <t>Wayve, a London-based autonomous driving technology company, is leading the way in AV 2.0, the next generation of self-driving cars. AV 2.0 focuses on comprehensive in-vehicle intelligence and uses generative AI to create and simulate novel driving scenarios. Wayve has developed GAIA-1, a generative world model, and LINGO-1, an AI model that enhances the learning and explainability of AI driving models. The company aims to improve the safety of autonomous vehicles and believes that embodied AI will play a definitive role in the future of the AI landscape.</t>
-  </si>
-  <si>
-    <t>The AWS Machine Learning Blog discusses the potential of generative AI to transform customer experiences and businesses. AWS offers a comprehensive set of capabilities across the three layers of the generative AI stack: infrastructure for training models, easy access to models and tools, and game-changing applications. AWS has introduced new capabilities, such as AWS Trainium2 for training large-scale models, and Amazon Bedrock, which allows customers to choose from industry-leading models and customize them with their own data. Additionally, AWS offers Amazon CodeWhisperer for AI-based coding and Amazon Q, a generative AI-powered assistant tailored for work.</t>
-  </si>
-  <si>
-    <t>Microsoft Cloud for Sovereignty is now generally available across all Azure regions. This cloud service helps governments meet compliance, security, and policy requirements while utilizing the cloud for innovation. It offers governance, security, transparency, and sovereign technology, allowing customers to implement policies to contain their data within their preferred geographic boundary. Microsoft Cloud for Sovereignty also provides sovereign controls to protect and encrypt sensitive data and offers specific Azure policy initiatives to address national and regional regulatory requirements. The service is already being used by organizations such as the National Cyber Security Center in the Netherlands and the municipality of Amsterdam. Microsoft is also introducing new capabilities, including drift analysis capabilities and transparency logs, to further enhance sovereignty in the hyperscale cloud.</t>
-  </si>
-  <si>
-    <t>OpenAI is conducting research to develop artificial general intelligence (AGI) that can solve human-level problems. They are focused on aligning powerful AI systems with human intentions and are using deep learning to build generative models for text, images, and audio. Their research has led to advancements in language processing, image generation, and audio processing. OpenAI has also developed tools like CLIP and DALL-E for connecting text and images. They are actively seeking talented individuals to join their team.</t>
-  </si>
-  <si>
-    <t>The European Union (EU) is expanding its support for AI startups by providing them with access to its supercomputers for model training. The EU plans to set up "centers of excellence" to support the development of dedicated AI algorithms that can run on its supercomputers. The program aims to help AI startups learn how to best utilize the computing power of the supercomputers. The EU sees AI as a strategic priority and wants to provide innovation capacity for SMEs and startups to develop safe and ethical AI algorithms. The EU is also planning to acquire quantum simulators to combine with supercomputers for hybrid computing. The EU's supercomputing resources are being used for various applications, including simulating Earth's ecosystems and creating a digital twin of the human body. The EU's support for AI startups aligns with its goal of fostering a competitive AI ecosystem in Europe.</t>
-  </si>
-  <si>
-    <t>The paper titled "ProlificDreamer: High-Fidelity and Diverse Text-to-3D Generation with Variational Score Distillation" proposes a new approach called variational score distillation (VSD) to improve text-to-3D generation. The current method, score distillation sampling (SDS), suffers from issues such as over-saturation, over-smoothing, and low diversity. VSD models the 3D parameter as a random variable and addresses these issues by using a particle-based variational framework. The proposed approach, ProlificDreamer, generates high-resolution and high-fidelity 3D models with rich structure and complex effects. The paper also explores improvements in the design space for text-to-3D generation.</t>
-  </si>
-  <si>
-    <t>Intel has released its fifth-generation Xeon Scalable processors, which are designed to accelerate AI workloads. The new processors offer improved performance and efficiency, with up to 64 cores and AI acceleration capabilities in each core. They also feature Intel AMX, a dedicated matrix computing unit for AI acceleration. The processors have been validated by companies such as JD Cloud and Alibaba Cloud, which have reported significant performance improvements in AI workloads. Intel is also focusing on software support, providing tools like the oneAPI Deep Neural Network Library and OpenVINO toolkit to optimize and deploy AI models on its processors. The company is already working on the next generation of Xeon processors, which will have different core architectures to cater to different workloads.</t>
-  </si>
-  <si>
-    <t>The paper proposes a weakly supervised open-vocabulary object detection framework called WSOVOD. This framework extends traditional weakly supervised object detection (WSOD) to detect novel concepts and utilize diverse datasets with only image-level annotations. The authors explore three strategies: dataset-level feature adaptation, image-level salient object localization, and region-level vision-language alignment. Experimental results show that WSOVOD achieves state-of-the-art performance in both close-set object localization and detection tasks, and it also enables cross-dataset and open-vocabulary learning.</t>
-  </si>
-  <si>
-    <t>The paper discusses the issue of neglecting the correlation between timesteps in training methods for Denoising Probabilistic Models (DPMs), which limits their performance in generating images effectively. The authors propose a novel loss function that aims to reduce the estimation gap and enhance the sampling quality. Experimental results show that their method improves image generalization quality compared to several DPM baselines.</t>
-  </si>
-  <si>
-    <t>The article discusses the use of cloud technology and artificial intelligence (AI) in the field of radiology and medical imaging. It highlights how these advancements can improve the efficiency and accuracy of diagnoses, as well as the potential benefits of using cloud-based platforms for storing and sharing medical images.</t>
-  </si>
-  <si>
-    <t>The RSNA 2023 conference has attracted over 40,000 registrants, according to Google News.</t>
+    <t>论文《Bootstrap Your Own Variance》提出了一种名为BYOV的方法，将Bootstrap Your Own Latent（BYOL）与Bayes by Backprop（BBB）结合起来，用于评估模型的不确定性。作者发现，相比于确定性的BYOL基线，BYOV方法改进了模型的校准性和可靠性，在各种数据增强测试中展现出更好的性能。该论文经过了严格的审查，并成功发表在NeurIPS 2023自监督学习-理论与实践研讨会上。</t>
+  </si>
+  <si>
+    <t>总部位于伦敦的自动驾驶技术公司Wayve在AV 2.0领域处于领先地位。AV 2.0专注于车内智能，并利用生成式人工智能来模拟不同的驾驶场景。Wayve开发了GAIA-1生成世界模型和LINGO-1 AI模型，用于增强AI驾驶模型的学习和可解释性。该公司的目标是提升自动驾驶车辆的安全性，并相信实体化的人工智能在未来的发展中将扮演重要角色。</t>
+  </si>
+  <si>
+    <t>AWS机器学习博客讨论了生成式人工智能（generative AI）对客户体验和商业的潜力带来的变革。AWS为客户提供了一整套生成式AI堆栈能力，其中包括基础设施用于训练模型、易于访问的模型和工具，以及具有颠覆性应用的能力。AWS还推出了一些新功能，如用于训练大规模模型的AWS Trainium2和Amazon Bedrock，使客户能够选择行业领先的模型并进行个性化定制。此外，AWS还提供了基于AI的编码工具Amazon CodeWhisperer和面向工作的生成式AI助手Amazon Q。总的来说，AWS正在致力于构建强大的生成式人工智能平台，以满足客户不断增长的需求。</t>
+  </si>
+  <si>
+    <t>Microsoft Cloud for Sovereignty是Azure云服务的一部分。该服务旨在帮助政府满足合规性、安全性和政策要求，并在创新中利用云服务。这项服务提供了治理、安全、透明度和主权技术，允许客户在他们首选的地理范围内实施数据约束政策。Microsoft Cloud for Sovereignty还提供主权控制，以保护和加密敏感数据，并提供特定的Azure策略倡议，以满足国家和地区的监管要求。目前，该服务已在荷兰、意大利和比利时的政府机构中得到应用。微软还推出了新的功能，如漂移分析工具和透明度日志，以进一步增强超大规模云的主权性能。该服务为政府部门提供了一个安全、合规和可靠的云解决方案。</t>
+  </si>
+  <si>
+    <t>OpenAI是一家致力于开发通用人工智能（AGI）的研究机构。他们的目标是构建具备类人级别问题解决能力的强大人工智能系统，并且与人类意图保持一致。为了实现这一目标，他们运用了深度学习技术来构建文本、图像和音频的生成模型。在语言处理、图像生成和音频处理方面，OpenAI的研究取得了显著进展。同时，他们还开发了多个工具，如CLIP和DALL-E，用于将文本与图像相连接。为了推动研究和发展，OpenAI正在积极招募具备才能的人才加入他们的团队。通过这些努力，OpenAI致力于推动人工智能技术的发展，并为社会带来更多的创新和应用。</t>
+  </si>
+  <si>
+    <t>欧盟正在加大对人工智能初创企业的支持力度，提供使用超级计算机进行模型训练的机会。他们计划建立“卓越中心”，帮助初创企业学会如何充分利用超级计算机的计算能力。欧盟把人工智能视为战略重点，希望为中小企业和初创企业提供创新能力，开发安全和道德的人工智能算法。此外，欧盟还计划结合超级计算机和量子模拟器，实现混合计算。超级计算资源在欧盟被广泛应用，包括模拟地球生态系统和创建人体的数字孪生。欧盟的支持与培育竞争性人工智能生态系统的目标是一致的。</t>
+  </si>
+  <si>
+    <t>这篇题为《ProlificDreamer: 使用变分分数蒸馏的高保真度和多样性文本到3D生成》的论文提出了一种名为变分分数蒸馏（VSD）的新方法来改善文本到3D生成。VSD将3D参数建模为随机变量，并通过使用基于粒子的变分框架来解决分数蒸馏采样（SDS）存在的过饱和、过平滑和低多样性等问题。通过ProlificDreamer生成的3D模型具有高分辨率、高保真度，并呈现出丰富的结构和复杂的效果。论文还对文本到3D生成的设计空间进行了改进探索。</t>
+  </si>
+  <si>
+    <t>腾讯AI实验室的游戏AI团队通过对《星际争霸II》游戏中决策AI“决武”的研究取得了突破。他们创新性地开发了一种训练方法，显著提升了AI在游戏策略方面的适应能力。在与三名顶级职业选手对战时，该AI保持了50%或更高的胜率。这项研究对于推动AI智能发展，提高其处理复杂问题的能力具有重要贡献。团队采用了目标条件强化学习技术来提高AI的训练效果，并引入对手建模来增强其适应不同对手策略的能力。研究结果表明该AI展现了出色的策略适应性和稳健性。</t>
+  </si>
+  <si>
+    <t>本文介绍了云技术和人工智能在放射学和医学成像领域的应用。研究表明，这些技术的发展可以显著提高诊断的效率和准确性，为医生提供更好的决策支持。另外，利用云平台存储和共享医学图像的好处也被强调。云存储可以提供安全可靠的数据存储，同时实现图像的快速访问和共享，方便多学科团队的合作和远程会诊。然而，文章指出，在应用云技术和人工智能时，仍需注意数据隐私和安全问题，并制定相应的政策和规范来保护患者的个人信息。总的来说，云技术和人工智能的应用对医学诊断和成像具有重要推动作用，但同时需综合考虑技术和伦理问题。</t>
+  </si>
+  <si>
+    <t>根据Google新闻报道，RSNA 2023会议已经吸引了超过40,000名注册参会者。</t>
   </si>
 </sst>
 </file>
@@ -535,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -560,13 +538,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -574,13 +552,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -588,13 +566,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -602,13 +580,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -616,13 +594,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -630,13 +608,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -644,13 +622,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -658,13 +636,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -672,57 +650,30 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -735,8 +686,6 @@
     <hyperlink ref="C9" r:id="rId8"/>
     <hyperlink ref="C10" r:id="rId9"/>
     <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
use func to do md generation
</commit_message>
<xml_diff>
--- a/web_sum_output.xlsx
+++ b/web_sum_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>URL</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Title</t>
   </si>
   <si>
+    <t>google</t>
+  </si>
+  <si>
     <t>apple</t>
   </si>
   <si>
@@ -52,37 +55,47 @@
     <t>机器之心</t>
   </si>
   <si>
-    <t>google</t>
-  </si>
-  <si>
-    <t>自我引导，迎接变化</t>
-  </si>
-  <si>
-    <t>自动驾驶汽车的下一个重要创新方式：AV 2.0</t>
-  </si>
-  <si>
-    <t>基于AWS的云端生成式AI建筑</t>
-  </si>
-  <si>
-    <t>微软主权云正式推出，为政府创新铺就新路径</t>
-  </si>
-  <si>
-    <t>通向人工智能通用智能之路的先驱性研究</t>
-  </si>
-  <si>
-    <t>欧盟扩大对人工智能初创公司的支持，利用超级计算机进行模型训练</t>
-  </si>
-  <si>
-    <t>高保真度和多样性的文本到3D生成技术</t>
-  </si>
-  <si>
-    <t>腾讯AI Lab在星际争霸2中对职业选手应用灵活策略：NeurIPS 2023焦点报告</t>
-  </si>
-  <si>
-    <t>放射学邂逅云端技术：探索健康影像的未来！</t>
-  </si>
-  <si>
-    <t>RSNA 2023大会吸引超过40000名注册者</t>
+    <t>Unveiling Evolving Trends In Medical Imaging - MedTech Outlook</t>
+  </si>
+  <si>
+    <t>If AI is the future, radiology needs to look to the cloud - Health Imaging</t>
+  </si>
+  <si>
+    <t>RSNA 2023 Draws Over 40000 Registrants - Imaging Technology News</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bootstrap Your Own Variance </t>
+  </si>
+  <si>
+    <t>AV 2.0, the Next Big Wayve in Self-Driving Cars</t>
+  </si>
+  <si>
+    <t>Welcome to a New Era of Building in the Cloud with Generative AI on AWS</t>
+  </si>
+  <si>
+    <t>Microsoft Cloud for Sovereignty now generally available, opening new pathways for government innovation</t>
+  </si>
+  <si>
+    <t>Pioneering research on the path to AGI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+				EU to expand support for AI startups to tap its supercomputers for model training			</t>
+  </si>
+  <si>
+    <t>ProlificDreamer: High-Fidelity and Diverse Text-to-3D Generation with Variational Score Distillation</t>
+  </si>
+  <si>
+    <t>大模型+搜索构建完整技术栈，百川智能用搜索增强给企业定制化下了一剂「猛药」</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMiY2h0dHBzOi8vd3d3Lm1lZGljYWx0ZWNob3V0bG9vay5jb20vbmV3cy91bnZlaWxpbmctZXZvbHZpbmctdHJlbmRzLWluLW1lZGljYWwtaW1hZ2luZy1ud2lkLTMxNzMuaHRtbNIBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMiYGh0dHBzOi8vaGVhbHRoaW1hZ2luZy5jb20vdG9waWNzL2hlYWx0aC1pdC9lbnRlcnByaXNlLWltYWdpbmcvcmFkaW9sb2d5LWNsb3VkLW1lZGljYWwtaW1hZ2luZy1hadIBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
+  </si>
+  <si>
+    <t>https://news.google.com/rss/articles/CBMiSGh0dHBzOi8vd3d3Lml0bm9ubGluZS5jb20vY29udGVudC9yc25hLTIwMjMtZHJhd3Mtb3Zlci00MDAwMC1yZWdpc3RyYW50c9IBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
   </si>
   <si>
     <t>https://machinelearning.apple.com//research/bootstrap-own-variance</t>
@@ -106,43 +119,40 @@
     <t>https://paperswithcode.com/paper/prolificdreamer-high-fidelity-and-diverse</t>
   </si>
   <si>
-    <t>https://www.jiqizhixin.com//articles/2023-12-20-5</t>
-  </si>
-  <si>
-    <t>https://news.google.com/rss/articles/CBMiYGh0dHBzOi8vaGVhbHRoaW1hZ2luZy5jb20vdG9waWNzL2hlYWx0aC1pdC9lbnRlcnByaXNlLWltYWdpbmcvcmFkaW9sb2d5LWNsb3VkLW1lZGljYWwtaW1hZ2luZy1hadIBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
-  </si>
-  <si>
-    <t>https://news.google.com/rss/articles/CBMiSGh0dHBzOi8vd3d3Lml0bm9ubGluZS5jb20vY29udGVudC9yc25hLTIwMjMtZHJhd3Mtb3Zlci00MDAwMC1yZWdpc3RyYW50c9IBAA?oc=5&amp;hl=en-US&amp;gl=US&amp;ceid=US:en</t>
-  </si>
-  <si>
-    <t>论文《Bootstrap Your Own Variance》提出了一种名为BYOV的方法，将Bootstrap Your Own Latent（BYOL）与Bayes by Backprop（BBB）结合起来，用于评估模型的不确定性。作者发现，相比于确定性的BYOL基线，BYOV方法改进了模型的校准性和可靠性，在各种数据增强测试中展现出更好的性能。该论文经过了严格的审查，并成功发表在NeurIPS 2023自监督学习-理论与实践研讨会上。</t>
-  </si>
-  <si>
-    <t>总部位于伦敦的自动驾驶技术公司Wayve在AV 2.0领域处于领先地位。AV 2.0专注于车内智能，并利用生成式人工智能来模拟不同的驾驶场景。Wayve开发了GAIA-1生成世界模型和LINGO-1 AI模型，用于增强AI驾驶模型的学习和可解释性。该公司的目标是提升自动驾驶车辆的安全性，并相信实体化的人工智能在未来的发展中将扮演重要角色。</t>
-  </si>
-  <si>
-    <t>AWS机器学习博客讨论了生成式人工智能（generative AI）对客户体验和商业的潜力带来的变革。AWS为客户提供了一整套生成式AI堆栈能力，其中包括基础设施用于训练模型、易于访问的模型和工具，以及具有颠覆性应用的能力。AWS还推出了一些新功能，如用于训练大规模模型的AWS Trainium2和Amazon Bedrock，使客户能够选择行业领先的模型并进行个性化定制。此外，AWS还提供了基于AI的编码工具Amazon CodeWhisperer和面向工作的生成式AI助手Amazon Q。总的来说，AWS正在致力于构建强大的生成式人工智能平台，以满足客户不断增长的需求。</t>
-  </si>
-  <si>
-    <t>Microsoft Cloud for Sovereignty是Azure云服务的一部分。该服务旨在帮助政府满足合规性、安全性和政策要求，并在创新中利用云服务。这项服务提供了治理、安全、透明度和主权技术，允许客户在他们首选的地理范围内实施数据约束政策。Microsoft Cloud for Sovereignty还提供主权控制，以保护和加密敏感数据，并提供特定的Azure策略倡议，以满足国家和地区的监管要求。目前，该服务已在荷兰、意大利和比利时的政府机构中得到应用。微软还推出了新的功能，如漂移分析工具和透明度日志，以进一步增强超大规模云的主权性能。该服务为政府部门提供了一个安全、合规和可靠的云解决方案。</t>
-  </si>
-  <si>
-    <t>OpenAI是一家致力于开发通用人工智能（AGI）的研究机构。他们的目标是构建具备类人级别问题解决能力的强大人工智能系统，并且与人类意图保持一致。为了实现这一目标，他们运用了深度学习技术来构建文本、图像和音频的生成模型。在语言处理、图像生成和音频处理方面，OpenAI的研究取得了显著进展。同时，他们还开发了多个工具，如CLIP和DALL-E，用于将文本与图像相连接。为了推动研究和发展，OpenAI正在积极招募具备才能的人才加入他们的团队。通过这些努力，OpenAI致力于推动人工智能技术的发展，并为社会带来更多的创新和应用。</t>
-  </si>
-  <si>
-    <t>欧盟正在加大对人工智能初创企业的支持力度，提供使用超级计算机进行模型训练的机会。他们计划建立“卓越中心”，帮助初创企业学会如何充分利用超级计算机的计算能力。欧盟把人工智能视为战略重点，希望为中小企业和初创企业提供创新能力，开发安全和道德的人工智能算法。此外，欧盟还计划结合超级计算机和量子模拟器，实现混合计算。超级计算资源在欧盟被广泛应用，包括模拟地球生态系统和创建人体的数字孪生。欧盟的支持与培育竞争性人工智能生态系统的目标是一致的。</t>
-  </si>
-  <si>
-    <t>这篇题为《ProlificDreamer: 使用变分分数蒸馏的高保真度和多样性文本到3D生成》的论文提出了一种名为变分分数蒸馏（VSD）的新方法来改善文本到3D生成。VSD将3D参数建模为随机变量，并通过使用基于粒子的变分框架来解决分数蒸馏采样（SDS）存在的过饱和、过平滑和低多样性等问题。通过ProlificDreamer生成的3D模型具有高分辨率、高保真度，并呈现出丰富的结构和复杂的效果。论文还对文本到3D生成的设计空间进行了改进探索。</t>
-  </si>
-  <si>
-    <t>腾讯AI实验室的游戏AI团队通过对《星际争霸II》游戏中决策AI“决武”的研究取得了突破。他们创新性地开发了一种训练方法，显著提升了AI在游戏策略方面的适应能力。在与三名顶级职业选手对战时，该AI保持了50%或更高的胜率。这项研究对于推动AI智能发展，提高其处理复杂问题的能力具有重要贡献。团队采用了目标条件强化学习技术来提高AI的训练效果，并引入对手建模来增强其适应不同对手策略的能力。研究结果表明该AI展现了出色的策略适应性和稳健性。</t>
-  </si>
-  <si>
-    <t>本文介绍了云技术和人工智能在放射学和医学成像领域的应用。研究表明，这些技术的发展可以显著提高诊断的效率和准确性，为医生提供更好的决策支持。另外，利用云平台存储和共享医学图像的好处也被强调。云存储可以提供安全可靠的数据存储，同时实现图像的快速访问和共享，方便多学科团队的合作和远程会诊。然而，文章指出，在应用云技术和人工智能时，仍需注意数据隐私和安全问题，并制定相应的政策和规范来保护患者的个人信息。总的来说，云技术和人工智能的应用对医学诊断和成像具有重要推动作用，但同时需综合考虑技术和伦理问题。</t>
-  </si>
-  <si>
-    <t>根据Google新闻报道，RSNA 2023会议已经吸引了超过40,000名注册参会者。</t>
+    <t>https://www.jiqizhixin.com//articles/2023-12-20-10</t>
+  </si>
+  <si>
+    <t>The article discusses the evolving trends in medical imaging, highlighting the advancements and innovations in the field.</t>
+  </si>
+  <si>
+    <t>The article discusses the use of cloud technology and artificial intelligence (AI) in the field of radiology and medical imaging. It highlights how these advancements can improve the efficiency and accuracy of diagnoses, as well as the potential benefits of using cloud-based platforms for storing and sharing medical images.</t>
+  </si>
+  <si>
+    <t>The RSNA 2023 conference has attracted over 40,000 registrants, according to Google News.</t>
+  </si>
+  <si>
+    <t>The paper "Bootstrap Your Own Variance" proposes a method called BYOV that combines Bootstrap Your Own Latent (BYOL) with Bayes by Backprop (BBB) to estimate model uncertainty. The authors find that BYOV improves upon the deterministic BYOL baseline and provides better calibration and reliability when tested with various augmentations. The paper was accepted at the workshop Self-Supervised Learning - Theory and Practice at NeurIPS 2023.</t>
+  </si>
+  <si>
+    <t>Wayve, a London-based autonomous driving technology company, is leading the way in AV 2.0, the next generation of self-driving cars. AV 2.0 focuses on comprehensive in-vehicle intelligence and uses generative AI to create and simulate novel driving scenarios. Wayve has developed GAIA-1, a generative world model, and LINGO-1, an AI model that enhances the learning and explainability of AI driving models. The company aims to improve the safety of autonomous vehicles and believes that embodied AI will play a crucial role in the future of the AI landscape.</t>
+  </si>
+  <si>
+    <t>The AWS Machine Learning Blog discusses the potential of generative AI to transform customer experiences and businesses. AWS offers a comprehensive set of capabilities across the three layers of the generative AI stack: infrastructure for training models, easy access to models and tools, and game-changing applications. AWS has introduced new capabilities, such as AWS Trainium2 for training large-scale models, and Amazon Bedrock, which allows customers to choose from industry-leading models and customize them with their own data. Additionally, AWS offers Amazon CodeWhisperer for AI-based coding and Amazon Q, a generative AI-powered assistant tailored for work.</t>
+  </si>
+  <si>
+    <t>Microsoft Cloud for Sovereignty is now generally available across all Azure regions. This cloud service helps governments meet compliance, security, and policy requirements while utilizing the cloud for innovation. It offers governance, security, transparency, and sovereign technology, allowing customers to implement policies to contain their data within their preferred geographic boundary. Microsoft Cloud for Sovereignty also provides sovereign controls to protect and encrypt sensitive data and offers specific Azure policy initiatives to address national and regional regulatory requirements. The service is already being used by organizations such as the National Cyber Security Center in the Netherlands and the municipality of Amsterdam. Microsoft is also introducing new capabilities, including drift analysis capabilities and transparency logs, to further enhance sovereignty in the hyperscale cloud.</t>
+  </si>
+  <si>
+    <t>OpenAI is conducting research to develop artificial general intelligence (AGI) that can solve human-level problems. They are focused on aligning powerful AI systems with human intentions and are using deep learning to build generative models for text, images, and audio. Their research has led to advancements in language processing, image generation, and audio processing. OpenAI has also developed tools like CLIP and DALL-E for connecting text and images. They are actively seeking talented individuals to join their team.</t>
+  </si>
+  <si>
+    <t>The European Union (EU) is expanding its support for AI startups by providing them with access to its supercomputers for model training. The EU plans to set up "centers of excellence" to support the development of dedicated AI algorithms that can run on its supercomputers. The program aims to help AI startups learn how to best utilize the computing power of the supercomputers. The EU sees AI as a strategic priority and wants to provide innovation capacity for SMEs and startups to develop safe and ethical AI algorithms. The EU is also planning to acquire quantum simulators to combine with supercomputers for hybrid computing. The EU's supercomputing resources are being used for various applications, including simulating Earth's ecosystems and creating a digital twin of the human body. The EU's support for AI startups aligns with its goal of fostering a competitive AI ecosystem in Europe.</t>
+  </si>
+  <si>
+    <t>The paper titled "ProlificDreamer: High-Fidelity and Diverse Text-to-3D Generation with Variational Score Distillation" proposes a new approach called variational score distillation (VSD) to improve text-to-3D generation. The current method, score distillation sampling (SDS), suffers from issues such as over-saturation, over-smoothing, and low diversity. VSD models the 3D parameter as a random variable and addresses these issues by using a particle-based variational framework. The proposed approach, ProlificDreamer, generates high-resolution and high-fidelity 3D models with rich structure and complex effects. The paper also explores improvements in the design space for text-to-3D generation.</t>
+  </si>
+  <si>
+    <t>Baichuan Intelligence has developed a "big model + search" technology stack that enhances customization for businesses. By combining a large model with a search function and the use of enterprise knowledge bases, Baichuan Intelligence aims to improve the accuracy and efficiency of AI applications. The company has released the Baichuan2-Turbo series API, which supports long context windows and the ability to upload specific text data to build customized knowledge bases. This approach allows for better integration of industry knowledge and addresses the challenges of applying large models to specific business scenarios. The combination of a long context window and search enhancement improves the application potential of large models by providing more accurate and comprehensive information processing. Baichuan Intelligence's approach has shown promising results in accuracy testing and outperforms industry-leading models in various tasks. The integration of a large model with search capabilities opens up new possibilities for customized AI solutions in various industries.</t>
   </si>
 </sst>
 </file>
@@ -513,7 +523,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -541,139 +551,151 @@
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A2:A4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -686,6 +708,7 @@
     <hyperlink ref="C9" r:id="rId8"/>
     <hyperlink ref="C10" r:id="rId9"/>
     <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>